<commit_message>
CREATE TABLE without column types
</commit_message>
<xml_diff>
--- a/test/test251.xlsx
+++ b/test/test251.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4" t="str">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C4" t="str">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D4" t="str">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -460,17 +460,6 @@
         <v>SECOND(NOW())</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>7</v>
-      </c>
-      <c r="B6" t="str">
-        <v>36</v>
-      </c>
-      <c r="C6" t="str">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved problem with index in test250.js. Still problem with batch testing accurs
</commit_message>
<xml_diff>
--- a/test/test251.xlsx
+++ b/test/test251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4" t="str">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" t="str">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Convert CRLF to LF
</commit_message>
<xml_diff>
--- a/test/test251.xlsx
+++ b/test/test251.xlsx
@@ -443,10 +443,10 @@
         <v>22</v>
       </c>
       <c r="C4" t="str">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D4" t="str">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Fixed bug with localStorage DELETE FROM
</commit_message>
<xml_diff>
--- a/test/test251.xlsx
+++ b/test/test251.xlsx
@@ -443,10 +443,10 @@
         <v>21</v>
       </c>
       <c r="C4" t="str">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D4" t="str">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Changed tests to 'res*'
</commit_message>
<xml_diff>
--- a/test/test251.xlsx
+++ b/test/test251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>